<commit_message>
Newest version of Logic Module V3
</commit_message>
<xml_diff>
--- a/Hardware/Electrical Components/Module - Logic/Logic Module V3/BOM Logic Module V3.xlsx
+++ b/Hardware/Electrical Components/Module - Logic/Logic Module V3/BOM Logic Module V3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{3B485AB5-865B-4FE1-A814-5ACCF61F15D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC05A65A-B3FD-4D1E-8866-37F02E419D1D}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{3B485AB5-865B-4FE1-A814-5ACCF61F15D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CE7EE05-DC7D-46C7-8DE8-3C67D8188FC4}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1176" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="84">
   <si>
     <t>Digikey</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>311-39KERCT-ND</t>
+  </si>
+  <si>
+    <t>V3 INV</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>Ordered</t>
   </si>
 </sst>
 </file>
@@ -454,7 +463,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -594,6 +603,10 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -879,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B52106-704B-42A8-8108-9AAA1C03317C}">
   <dimension ref="A2:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,6 +930,9 @@
       <c r="H2" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="J2" s="61" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -939,6 +955,9 @@
         <f>F3*D3</f>
         <v>3.3</v>
       </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
@@ -960,6 +979,9 @@
       <c r="G4" s="10">
         <f t="shared" ref="G4:G27" si="0">F4*D4</f>
         <v>1.58</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -983,6 +1005,9 @@
         <f t="shared" si="0"/>
         <v>0.62</v>
       </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -1005,6 +1030,9 @@
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
@@ -1027,6 +1055,9 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -1049,6 +1080,9 @@
         <f t="shared" ref="G8" si="1">F8*D8</f>
         <v>0.51</v>
       </c>
+      <c r="J8" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="44" t="s">
@@ -1076,7 +1110,9 @@
       <c r="I9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="55">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -1098,6 +1134,9 @@
       <c r="G10" s="31">
         <f>F10*D10</f>
         <v>0.2</v>
+      </c>
+      <c r="J10" s="62">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1130,6 +1169,9 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
@@ -1152,6 +1194,9 @@
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
+      <c r="J13" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -1174,6 +1219,9 @@
         <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
@@ -1196,6 +1244,9 @@
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
@@ -1218,8 +1269,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="25" t="s">
         <v>0</v>
@@ -1240,8 +1294,11 @@
         <f t="shared" si="0"/>
         <v>0.37</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="25" t="s">
         <v>0</v>
@@ -1262,8 +1319,11 @@
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="25" t="s">
         <v>0</v>
@@ -1284,8 +1344,11 @@
         <f t="shared" si="0"/>
         <v>1.44</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="25" t="s">
         <v>0</v>
@@ -1306,8 +1369,11 @@
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="25" t="s">
         <v>0</v>
@@ -1328,8 +1394,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="18" t="s">
         <v>0</v>
@@ -1350,8 +1419,11 @@
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="18" t="s">
         <v>0</v>
@@ -1372,8 +1444,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="25" t="s">
         <v>0</v>
@@ -1394,8 +1469,11 @@
         <f t="shared" si="0"/>
         <v>1.24</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="25" t="s">
         <v>0</v>
@@ -1416,8 +1494,11 @@
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="26" t="s">
         <v>0</v>
@@ -1438,8 +1519,11 @@
         <f>F26*D26</f>
         <v>0.76</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J26" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="25" t="s">
         <v>0</v>
@@ -1460,8 +1544,11 @@
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="25" t="s">
         <v>0</v>
@@ -1482,8 +1569,11 @@
         <f>F28*D28</f>
         <v>0.32</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="52"/>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -1492,7 +1582,7 @@
       <c r="F29" s="53"/>
       <c r="G29" s="53"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="48"/>
       <c r="B30" s="23" t="s">
         <v>0</v>
@@ -1517,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48"/>
       <c r="B31" s="58" t="s">
         <v>0</v>
@@ -1539,7 +1629,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="48"/>
       <c r="B32" s="58" t="s">
         <v>0</v>
@@ -1561,7 +1651,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="48"/>
       <c r="B33" s="58" t="s">
         <v>0</v>
@@ -1583,7 +1673,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="48"/>
       <c r="B34" s="58" t="s">
         <v>0</v>
@@ -1605,7 +1695,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="22" t="s">
         <v>0</v>
@@ -1627,7 +1717,7 @@
         <v>8.77</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="26" t="s">
         <v>0</v>
@@ -1648,8 +1738,11 @@
         <f t="shared" ref="G36:G37" si="4">F36*D36</f>
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
       <c r="B37" s="25" t="s">
         <v>0</v>
@@ -1670,16 +1763,22 @@
         <f t="shared" si="4"/>
         <v>1.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>50</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
         <v>51</v>
       </c>
@@ -1687,12 +1786,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F41" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>